<commit_message>
Removed one insignificant row from dataset
</commit_message>
<xml_diff>
--- a/student_dataset.xlsx
+++ b/student_dataset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Roll No</t>
   </si>
@@ -321,12 +321,6 @@
   </si>
   <si>
     <t>TRIVEDI MANAN HIMANSHU</t>
-  </si>
-  <si>
-    <t>214a1113</t>
-  </si>
-  <si>
-    <t>AMBAT SHRINIVAS RAMESH MEENAKSHI</t>
   </si>
   <si>
     <t>214a1114</t>
@@ -834,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -862,28 +856,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6">
@@ -2203,7 +2197,7 @@
         <v>84</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C43" s="9">
         <v>60</v>
@@ -2394,63 +2388,31 @@
       <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="9">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D49" s="20">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E49" s="9">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F49" s="20">
-        <v>39</v>
-      </c>
-      <c r="G49" s="8">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="G49" s="9">
+        <v>67</v>
       </c>
       <c r="H49" s="20">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I49" s="9">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="J49" s="20">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="31.2">
-      <c r="A50" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="9">
-        <v>45</v>
-      </c>
-      <c r="D50" s="20">
-        <v>10</v>
-      </c>
-      <c r="E50" s="9">
-        <v>35</v>
-      </c>
-      <c r="F50" s="20">
-        <v>32</v>
-      </c>
-      <c r="G50" s="9">
-        <v>67</v>
-      </c>
-      <c r="H50" s="20">
-        <v>32</v>
-      </c>
-      <c r="I50" s="9">
-        <v>55</v>
-      </c>
-      <c r="J50" s="20">
         <v>41</v>
       </c>
     </row>

</xml_diff>